<commit_message>
Made some final changes, got everything working perfect! (for now)
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jared Rutherford\Gemini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>TIME</t>
   </si>
@@ -144,6 +144,10 @@
   </si>
   <si>
     <t>Oct 16th - 9:30 to 11:50; 17th - 10 to 11</t>
+  </si>
+  <si>
+    <t>Oct 16th - 6 to 7
+Oct 18th - 7 to 12</t>
   </si>
 </sst>
 </file>
@@ -235,12 +239,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -251,6 +258,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -635,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -652,26 +665,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -686,10 +699,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
@@ -702,75 +715,148 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="3">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.25</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>